<commit_message>
Some data wrangling on the population ticket excel file.
</commit_message>
<xml_diff>
--- a/analysis/census-demographics/commarea-population-w-tickets.xlsx
+++ b/analysis/census-demographics/commarea-population-w-tickets.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="22420" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="22420" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="2014pop" sheetId="1" r:id="rId1"/>
@@ -1480,8 +1480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H469"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
@@ -4698,8 +4698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A46" sqref="A46:XFD46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -4759,42 +4759,42 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C2">
-        <v>98514</v>
+        <v>18001</v>
       </c>
       <c r="D2">
-        <v>573</v>
+        <v>8</v>
       </c>
       <c r="E2">
-        <v>83837</v>
+        <v>17315</v>
       </c>
       <c r="F2">
-        <v>8722</v>
+        <v>348</v>
       </c>
       <c r="G2">
-        <v>4364</v>
+        <v>133</v>
       </c>
       <c r="H2">
-        <v>1018</v>
+        <v>197</v>
       </c>
       <c r="I2" s="12">
-        <v>1284</v>
+        <v>613</v>
       </c>
       <c r="J2" s="14">
-        <v>676</v>
+        <v>2</v>
       </c>
       <c r="K2">
         <f>(I2/C2)*10000</f>
-        <v>130.33680492112796</v>
+        <v>340.53663685350818</v>
       </c>
       <c r="L2">
         <f>(J2/C2)*10000</f>
-        <v>68.619688572182639</v>
+        <v>1.1110493861452142</v>
       </c>
       <c r="M2" t="s">
         <v>173</v>
@@ -4802,42 +4802,42 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="C3">
-        <v>52010</v>
+        <v>35912</v>
       </c>
       <c r="D3">
-        <v>124</v>
+        <v>74</v>
       </c>
       <c r="E3">
-        <v>49338</v>
+        <v>32835</v>
       </c>
       <c r="F3">
-        <v>893</v>
+        <v>2144</v>
       </c>
       <c r="G3">
-        <v>724</v>
+        <v>492</v>
       </c>
       <c r="H3">
-        <v>931</v>
+        <v>367</v>
       </c>
       <c r="I3" s="12">
-        <v>567</v>
+        <v>1023</v>
       </c>
       <c r="J3" s="12">
-        <v>102</v>
+        <v>200</v>
       </c>
       <c r="K3">
         <f>(I3/C3)*10000</f>
-        <v>109.01749663526245</v>
+        <v>284.86299844063268</v>
       </c>
       <c r="L3">
         <f>(J3/C3)*10000</f>
-        <v>19.611613151317055</v>
+        <v>55.691690799732683</v>
       </c>
       <c r="M3" t="s">
         <v>173</v>
@@ -4845,42 +4845,42 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="C4">
-        <v>48743</v>
+        <v>31198</v>
       </c>
       <c r="D4">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="E4">
-        <v>47661</v>
+        <v>23296</v>
       </c>
       <c r="F4">
-        <v>459</v>
+        <v>6774</v>
       </c>
       <c r="G4">
-        <v>134</v>
+        <v>599</v>
       </c>
       <c r="H4">
-        <v>456</v>
+        <v>462</v>
       </c>
       <c r="I4" s="12">
-        <v>323</v>
+        <v>570</v>
       </c>
       <c r="J4" s="14">
-        <v>51</v>
+        <v>2</v>
       </c>
       <c r="K4">
         <f>(I4/C4)*10000</f>
-        <v>66.265925363641955</v>
+        <v>182.70401948842874</v>
       </c>
       <c r="L4">
         <f>(J4/C4)*10000</f>
-        <v>10.463040846890834</v>
+        <v>0.64106673504711842</v>
       </c>
       <c r="M4" t="s">
         <v>173</v>
@@ -4888,42 +4888,42 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="C5">
-        <v>44619</v>
+        <v>35505</v>
       </c>
       <c r="D5">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="E5">
-        <v>43447</v>
+        <v>34178</v>
       </c>
       <c r="F5">
-        <v>458</v>
+        <v>774</v>
       </c>
       <c r="G5">
-        <v>188</v>
+        <v>130</v>
       </c>
       <c r="H5">
-        <v>499</v>
+        <v>404</v>
       </c>
       <c r="I5" s="12">
-        <v>613</v>
+        <v>640</v>
       </c>
       <c r="J5" s="14">
-        <v>26</v>
+        <v>463</v>
       </c>
       <c r="K5">
         <f>(I5/C5)*10000</f>
-        <v>137.3854187677895</v>
+        <v>180.25630192930572</v>
       </c>
       <c r="L5">
         <f>(J5/C5)*10000</f>
-        <v>5.8271140097267979</v>
+        <v>130.4041684269821</v>
       </c>
       <c r="M5" t="s">
         <v>173</v>
@@ -4931,42 +4931,42 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>42</v>
       </c>
       <c r="C6">
-        <v>35505</v>
+        <v>11717</v>
       </c>
       <c r="D6">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E6">
-        <v>34178</v>
+        <v>11370</v>
       </c>
       <c r="F6">
-        <v>774</v>
+        <v>104</v>
       </c>
       <c r="G6">
-        <v>130</v>
+        <v>87</v>
       </c>
       <c r="H6">
-        <v>404</v>
+        <v>144</v>
       </c>
       <c r="I6" s="12">
-        <v>640</v>
+        <v>205</v>
       </c>
       <c r="J6" s="14">
-        <v>463</v>
+        <v>1</v>
       </c>
       <c r="K6">
         <f>(I6/C6)*10000</f>
-        <v>180.25630192930572</v>
+        <v>174.95946061278485</v>
       </c>
       <c r="L6">
         <f>(J6/C6)*10000</f>
-        <v>130.4041684269821</v>
+        <v>0.85346078347699927</v>
       </c>
       <c r="M6" t="s">
         <v>173</v>
@@ -4974,42 +4974,40 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="C7">
-        <v>35912</v>
+        <v>23740</v>
       </c>
       <c r="D7">
-        <v>74</v>
+        <v>544</v>
       </c>
       <c r="E7">
-        <v>32835</v>
+        <v>20605</v>
       </c>
       <c r="F7">
-        <v>2144</v>
+        <v>504</v>
       </c>
       <c r="G7">
-        <v>492</v>
+        <v>1623</v>
       </c>
       <c r="H7">
-        <v>367</v>
+        <v>464</v>
       </c>
       <c r="I7" s="12">
-        <v>1023</v>
-      </c>
-      <c r="J7" s="14">
-        <v>200</v>
-      </c>
+        <v>400</v>
+      </c>
+      <c r="J7" s="15"/>
       <c r="K7">
         <f>(I7/C7)*10000</f>
-        <v>284.86299844063268</v>
+        <v>168.49199663016006</v>
       </c>
       <c r="L7">
         <f>(J7/C7)*10000</f>
-        <v>55.691690799732683</v>
+        <v>0</v>
       </c>
       <c r="M7" t="s">
         <v>173</v>
@@ -5017,42 +5015,42 @@
     </row>
     <row r="8" spans="1:13">
       <c r="A8">
-        <v>69</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>73</v>
+        <v>27</v>
       </c>
       <c r="C8">
-        <v>32602</v>
+        <v>20567</v>
       </c>
       <c r="D8">
-        <v>21</v>
+        <v>83</v>
       </c>
       <c r="E8">
-        <v>31590</v>
+        <v>18696</v>
       </c>
       <c r="F8">
-        <v>388</v>
+        <v>850</v>
       </c>
       <c r="G8">
-        <v>180</v>
+        <v>698</v>
       </c>
       <c r="H8">
-        <v>423</v>
+        <v>240</v>
       </c>
       <c r="I8" s="12">
-        <v>279</v>
+        <v>333</v>
       </c>
       <c r="J8" s="12">
-        <v>21</v>
+        <v>474</v>
       </c>
       <c r="K8">
         <f>(I8/C8)*10000</f>
-        <v>85.577571928102572</v>
+        <v>161.90985559391257</v>
       </c>
       <c r="L8">
         <f>(J8/C8)*10000</f>
-        <v>6.4413226182442793</v>
+        <v>230.46628093547915</v>
       </c>
       <c r="M8" t="s">
         <v>173</v>
@@ -5060,85 +5058,85 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="C9">
-        <v>31028</v>
+        <v>56323</v>
       </c>
       <c r="D9">
-        <v>27</v>
+        <v>222</v>
       </c>
       <c r="E9">
-        <v>30160</v>
+        <v>23030</v>
       </c>
       <c r="F9">
-        <v>311</v>
+        <v>30046</v>
       </c>
       <c r="G9">
-        <v>112</v>
+        <v>2502</v>
       </c>
       <c r="H9">
-        <v>418</v>
+        <v>523</v>
       </c>
       <c r="I9" s="12">
-        <v>167</v>
+        <v>908</v>
       </c>
       <c r="J9" s="14">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="K9">
         <f>(I9/C9)*10000</f>
-        <v>53.822354002836143</v>
+        <v>161.21300356870194</v>
       </c>
       <c r="L9">
         <f>(J9/C9)*10000</f>
-        <v>2.900605904344463</v>
+        <v>2.6632104113772348</v>
       </c>
       <c r="M9" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="A10">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="C10">
-        <v>30654</v>
+        <v>44619</v>
       </c>
       <c r="D10">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E10">
-        <v>29847</v>
+        <v>43447</v>
       </c>
       <c r="F10">
-        <v>325</v>
+        <v>458</v>
       </c>
       <c r="G10">
-        <v>105</v>
+        <v>188</v>
       </c>
       <c r="H10">
-        <v>343</v>
+        <v>499</v>
       </c>
       <c r="I10" s="12">
-        <v>349</v>
+        <v>613</v>
       </c>
       <c r="J10" s="14">
-        <v>70</v>
+        <v>26</v>
       </c>
       <c r="K10">
         <f>(I10/C10)*10000</f>
-        <v>113.85137339335813</v>
+        <v>137.3854187677895</v>
       </c>
       <c r="L10">
         <f>(J10/C10)*10000</f>
-        <v>22.835519018725122</v>
+        <v>5.8271140097267979</v>
       </c>
       <c r="M10" t="s">
         <v>173</v>
@@ -5146,171 +5144,171 @@
     </row>
     <row r="11" spans="1:13">
       <c r="A11">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="C11">
-        <v>29651</v>
+        <v>44377</v>
       </c>
       <c r="D11">
-        <v>14</v>
+        <v>727</v>
       </c>
       <c r="E11">
-        <v>27593</v>
+        <v>13148</v>
       </c>
       <c r="F11">
-        <v>1509</v>
+        <v>25431</v>
       </c>
       <c r="G11">
-        <v>166</v>
+        <v>4697</v>
       </c>
       <c r="H11">
-        <v>369</v>
+        <v>374</v>
       </c>
       <c r="I11" s="12">
-        <v>292</v>
+        <v>590</v>
       </c>
       <c r="J11" s="12">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="K11">
         <f>(I11/C11)*10000</f>
-        <v>98.478972041415119</v>
+        <v>132.95175428713071</v>
       </c>
       <c r="L11">
         <f>(J11/C11)*10000</f>
-        <v>5.3961080570638424</v>
+        <v>13.971201297969669</v>
       </c>
       <c r="M11" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12">
-        <v>66</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>70</v>
+        <v>25</v>
       </c>
       <c r="C12">
-        <v>55628</v>
+        <v>98514</v>
       </c>
       <c r="D12">
-        <v>190</v>
+        <v>573</v>
       </c>
       <c r="E12">
-        <v>27403</v>
+        <v>83837</v>
       </c>
       <c r="F12">
-        <v>25141</v>
+        <v>8722</v>
       </c>
       <c r="G12">
-        <v>2419</v>
+        <v>4364</v>
       </c>
       <c r="H12">
-        <v>475</v>
+        <v>1018</v>
       </c>
       <c r="I12" s="12">
-        <v>722</v>
+        <v>1284</v>
       </c>
       <c r="J12" s="14">
-        <v>113</v>
+        <v>676</v>
       </c>
       <c r="K12">
         <f>(I12/C12)*10000</f>
-        <v>129.79075285827281</v>
+        <v>130.33680492112796</v>
       </c>
       <c r="L12">
         <f>(J12/C12)*10000</f>
-        <v>20.313511181419432</v>
+        <v>68.619688572182639</v>
       </c>
       <c r="M12" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B13" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C13">
-        <v>26493</v>
+        <v>55628</v>
       </c>
       <c r="D13">
-        <v>12</v>
+        <v>190</v>
       </c>
       <c r="E13">
-        <v>25793</v>
+        <v>27403</v>
       </c>
       <c r="F13">
-        <v>258</v>
+        <v>25141</v>
       </c>
       <c r="G13">
-        <v>121</v>
+        <v>2419</v>
       </c>
       <c r="H13">
-        <v>309</v>
+        <v>475</v>
       </c>
       <c r="I13" s="12">
-        <v>130</v>
+        <v>722</v>
       </c>
       <c r="J13" s="14">
-        <v>17</v>
+        <v>113</v>
       </c>
       <c r="K13">
         <f>(I13/C13)*10000</f>
-        <v>49.069565545615824</v>
+        <v>129.79075285827281</v>
       </c>
       <c r="L13">
         <f>(J13/C13)*10000</f>
-        <v>6.4167893405805305</v>
+        <v>20.313511181419432</v>
       </c>
       <c r="M13" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="C14">
-        <v>31198</v>
+        <v>30654</v>
       </c>
       <c r="D14">
-        <v>67</v>
+        <v>34</v>
       </c>
       <c r="E14">
-        <v>23296</v>
+        <v>29847</v>
       </c>
       <c r="F14">
-        <v>6774</v>
+        <v>325</v>
       </c>
       <c r="G14">
-        <v>599</v>
+        <v>105</v>
       </c>
       <c r="H14">
-        <v>462</v>
+        <v>343</v>
       </c>
       <c r="I14" s="12">
-        <v>570</v>
+        <v>349</v>
       </c>
       <c r="J14" s="12">
-        <v>2</v>
+        <v>70</v>
       </c>
       <c r="K14">
         <f>(I14/C14)*10000</f>
-        <v>182.70401948842874</v>
+        <v>113.85137339335813</v>
       </c>
       <c r="L14">
         <f>(J14/C14)*10000</f>
-        <v>0.64106673504711842</v>
+        <v>22.835519018725122</v>
       </c>
       <c r="M14" t="s">
         <v>173</v>
@@ -5318,85 +5316,85 @@
     </row>
     <row r="15" spans="1:13">
       <c r="A15">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="C15">
-        <v>56323</v>
+        <v>52010</v>
       </c>
       <c r="D15">
-        <v>222</v>
+        <v>124</v>
       </c>
       <c r="E15">
-        <v>23030</v>
+        <v>49338</v>
       </c>
       <c r="F15">
-        <v>30046</v>
+        <v>893</v>
       </c>
       <c r="G15">
-        <v>2502</v>
+        <v>724</v>
       </c>
       <c r="H15">
-        <v>523</v>
+        <v>931</v>
       </c>
       <c r="I15" s="12">
-        <v>908</v>
+        <v>567</v>
       </c>
       <c r="J15" s="14">
-        <v>15</v>
+        <v>102</v>
       </c>
       <c r="K15">
         <f>(I15/C15)*10000</f>
-        <v>161.21300356870194</v>
+        <v>109.01749663526245</v>
       </c>
       <c r="L15">
         <f>(J15/C15)*10000</f>
-        <v>2.6632104113772348</v>
+        <v>19.611613151317055</v>
       </c>
       <c r="M15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="16" spans="1:13">
       <c r="A16">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B16" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="C16">
-        <v>21929</v>
+        <v>29651</v>
       </c>
       <c r="D16">
-        <v>57</v>
+        <v>14</v>
       </c>
       <c r="E16">
-        <v>20645</v>
+        <v>27593</v>
       </c>
       <c r="F16">
-        <v>395</v>
+        <v>1509</v>
       </c>
       <c r="G16">
-        <v>391</v>
+        <v>166</v>
       </c>
       <c r="H16">
-        <v>441</v>
+        <v>369</v>
       </c>
       <c r="I16" s="12">
-        <v>190</v>
+        <v>292</v>
       </c>
       <c r="J16" s="14">
-        <v>193</v>
+        <v>16</v>
       </c>
       <c r="K16">
         <f>(I16/C16)*10000</f>
-        <v>86.643257786492768</v>
+        <v>98.478972041415119</v>
       </c>
       <c r="L16">
         <f>(J16/C16)*10000</f>
-        <v>88.011309225226881</v>
+        <v>5.3961080570638424</v>
       </c>
       <c r="M16" t="s">
         <v>173</v>
@@ -5404,126 +5402,128 @@
     </row>
     <row r="17" spans="1:13">
       <c r="A17">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C17">
-        <v>23740</v>
+        <v>79288</v>
       </c>
       <c r="D17">
-        <v>544</v>
+        <v>113</v>
       </c>
       <c r="E17">
-        <v>20605</v>
+        <v>10374</v>
       </c>
       <c r="F17">
-        <v>504</v>
+        <v>65457</v>
       </c>
       <c r="G17">
-        <v>1623</v>
+        <v>3056</v>
       </c>
       <c r="H17">
-        <v>464</v>
+        <v>288</v>
       </c>
       <c r="I17" s="12">
-        <v>400</v>
-      </c>
-      <c r="J17" s="15"/>
+        <v>760</v>
+      </c>
+      <c r="J17" s="14">
+        <v>17</v>
+      </c>
       <c r="K17">
         <f>(I17/C17)*10000</f>
-        <v>168.49199663016006</v>
+        <v>95.853092523458784</v>
       </c>
       <c r="L17">
         <f>(J17/C17)*10000</f>
-        <v>0</v>
+        <v>2.1440823327615779</v>
       </c>
       <c r="M17" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18" spans="1:13">
       <c r="A18">
-        <v>70</v>
+        <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="C18">
-        <v>41081</v>
+        <v>56362</v>
       </c>
       <c r="D18">
-        <v>276</v>
+        <v>6414</v>
       </c>
       <c r="E18">
-        <v>18976</v>
+        <v>11275</v>
       </c>
       <c r="F18">
-        <v>15132</v>
+        <v>8009</v>
       </c>
       <c r="G18">
-        <v>6251</v>
+        <v>29098</v>
       </c>
       <c r="H18">
-        <v>446</v>
+        <v>1566</v>
       </c>
       <c r="I18" s="12">
-        <v>38</v>
+        <v>517</v>
       </c>
       <c r="J18" s="14">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K18">
         <f>(I18/C18)*10000</f>
-        <v>9.2500182566149807</v>
+        <v>91.728469536212344</v>
       </c>
       <c r="L18">
         <f>(J18/C18)*10000</f>
-        <v>0.73026459920644582</v>
+        <v>1.064547035236507</v>
       </c>
       <c r="M18" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="19" spans="1:13">
       <c r="A19">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="C19">
-        <v>20567</v>
+        <v>21929</v>
       </c>
       <c r="D19">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="E19">
-        <v>18696</v>
+        <v>20645</v>
       </c>
       <c r="F19">
-        <v>850</v>
+        <v>395</v>
       </c>
       <c r="G19">
-        <v>698</v>
+        <v>391</v>
       </c>
       <c r="H19">
-        <v>240</v>
+        <v>441</v>
       </c>
       <c r="I19" s="12">
-        <v>333</v>
+        <v>190</v>
       </c>
       <c r="J19" s="14">
-        <v>474</v>
+        <v>193</v>
       </c>
       <c r="K19">
         <f>(I19/C19)*10000</f>
-        <v>161.90985559391257</v>
+        <v>86.643257786492768</v>
       </c>
       <c r="L19">
         <f>(J19/C19)*10000</f>
-        <v>230.46628093547915</v>
+        <v>88.011309225226881</v>
       </c>
       <c r="M19" t="s">
         <v>173</v>
@@ -5531,343 +5531,343 @@
     </row>
     <row r="20" spans="1:13">
       <c r="A20">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="C20">
-        <v>18001</v>
+        <v>54991</v>
       </c>
       <c r="D20">
-        <v>8</v>
+        <v>3523</v>
       </c>
       <c r="E20">
-        <v>17315</v>
+        <v>14461</v>
       </c>
       <c r="F20">
-        <v>348</v>
+        <v>13433</v>
       </c>
       <c r="G20">
-        <v>133</v>
+        <v>21618</v>
       </c>
       <c r="H20">
-        <v>197</v>
+        <v>1956</v>
       </c>
       <c r="I20" s="12">
-        <v>613</v>
+        <v>476</v>
       </c>
       <c r="J20" s="14">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="K20">
         <f>(I20/C20)*10000</f>
-        <v>340.53663685350818</v>
+        <v>86.559618846720369</v>
       </c>
       <c r="L20">
         <f>(J20/C20)*10000</f>
-        <v>1.1110493861452142</v>
+        <v>2.5458711425505993</v>
       </c>
       <c r="M20" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="21" spans="1:13">
       <c r="A21">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
+        <v>73</v>
       </c>
       <c r="C21">
-        <v>54881</v>
+        <v>32602</v>
       </c>
       <c r="D21">
-        <v>8022</v>
+        <v>21</v>
       </c>
       <c r="E21">
-        <v>17303</v>
+        <v>31590</v>
       </c>
       <c r="F21">
-        <v>5048</v>
+        <v>388</v>
       </c>
       <c r="G21">
-        <v>23042</v>
+        <v>180</v>
       </c>
       <c r="H21">
-        <v>1466</v>
+        <v>423</v>
       </c>
       <c r="I21" s="12">
-        <v>247</v>
+        <v>279</v>
       </c>
       <c r="J21" s="14">
-        <v>727</v>
+        <v>21</v>
       </c>
       <c r="K21">
         <f>(I21/C21)*10000</f>
-        <v>45.006468541025122</v>
+        <v>85.577571928102572</v>
       </c>
       <c r="L21">
         <f>(J21/C21)*10000</f>
-        <v>132.46843169767314</v>
+        <v>6.4413226182442793</v>
       </c>
       <c r="M21" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="22" spans="1:13">
       <c r="A22">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B22" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C22">
-        <v>22544</v>
+        <v>56521</v>
       </c>
       <c r="D22">
-        <v>92</v>
+        <v>6582</v>
       </c>
       <c r="E22">
-        <v>15039</v>
+        <v>8104</v>
       </c>
       <c r="F22">
-        <v>619</v>
+        <v>9318</v>
       </c>
       <c r="G22">
-        <v>6473</v>
+        <v>30889</v>
       </c>
       <c r="H22">
-        <v>321</v>
+        <v>1628</v>
       </c>
       <c r="I22" s="12">
-        <v>103</v>
+        <v>447</v>
       </c>
       <c r="J22" s="14">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="K22">
         <f>(I22/C22)*10000</f>
-        <v>45.688431511710434</v>
+        <v>79.08564958157146</v>
       </c>
       <c r="L22">
         <f>(J22/C22)*10000</f>
-        <v>1.3307310149041873</v>
+        <v>7.7847171847631857</v>
       </c>
       <c r="M22" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="23" spans="1:13">
       <c r="A23">
-        <v>1</v>
+        <v>71</v>
       </c>
       <c r="B23" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
       <c r="C23">
-        <v>54991</v>
+        <v>48743</v>
       </c>
       <c r="D23">
-        <v>3523</v>
+        <v>33</v>
       </c>
       <c r="E23">
-        <v>14461</v>
+        <v>47661</v>
       </c>
       <c r="F23">
-        <v>13433</v>
+        <v>459</v>
       </c>
       <c r="G23">
-        <v>21618</v>
+        <v>134</v>
       </c>
       <c r="H23">
-        <v>1956</v>
+        <v>456</v>
       </c>
       <c r="I23" s="12">
-        <v>476</v>
+        <v>323</v>
       </c>
       <c r="J23" s="14">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="K23">
         <f>(I23/C23)*10000</f>
-        <v>86.559618846720369</v>
+        <v>66.265925363641955</v>
       </c>
       <c r="L23">
         <f>(J23/C23)*10000</f>
-        <v>2.5458711425505993</v>
+        <v>10.463040846890834</v>
       </c>
       <c r="M23" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="24" spans="1:13">
       <c r="A24">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C24">
-        <v>18238</v>
+        <v>29283</v>
       </c>
       <c r="D24">
-        <v>2313</v>
+        <v>4658</v>
       </c>
       <c r="E24">
-        <v>13247</v>
+        <v>3361</v>
       </c>
       <c r="F24">
-        <v>465</v>
+        <v>2010</v>
       </c>
       <c r="G24">
-        <v>1810</v>
+        <v>18359</v>
       </c>
       <c r="H24">
-        <v>403</v>
+        <v>895</v>
       </c>
       <c r="I24" s="12">
-        <v>90</v>
+        <v>170</v>
       </c>
       <c r="J24" s="14">
-        <v>81</v>
+        <v>241</v>
       </c>
       <c r="K24">
         <f>(I24/C24)*10000</f>
-        <v>49.347516175019187</v>
+        <v>58.054161117371855</v>
       </c>
       <c r="L24">
         <f>(J24/C24)*10000</f>
-        <v>44.412764557517271</v>
+        <v>82.300310760509504</v>
       </c>
       <c r="M24" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="25" spans="1:13">
       <c r="A25">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="B25" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="C25">
-        <v>44377</v>
+        <v>31028</v>
       </c>
       <c r="D25">
-        <v>727</v>
+        <v>27</v>
       </c>
       <c r="E25">
-        <v>13148</v>
+        <v>30160</v>
       </c>
       <c r="F25">
-        <v>25431</v>
+        <v>311</v>
       </c>
       <c r="G25">
-        <v>4697</v>
+        <v>112</v>
       </c>
       <c r="H25">
-        <v>374</v>
+        <v>418</v>
       </c>
       <c r="I25" s="12">
-        <v>590</v>
+        <v>167</v>
       </c>
       <c r="J25" s="14">
-        <v>62</v>
+        <v>9</v>
       </c>
       <c r="K25">
         <f>(I25/C25)*10000</f>
-        <v>132.95175428713071</v>
+        <v>53.822354002836143</v>
       </c>
       <c r="L25">
         <f>(J25/C25)*10000</f>
-        <v>13.971201297969669</v>
+        <v>2.900605904344463</v>
       </c>
       <c r="M25" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="26" spans="1:13">
       <c r="A26">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>50</v>
+        <v>83</v>
       </c>
       <c r="C26">
-        <v>13812</v>
+        <v>80484</v>
       </c>
       <c r="D26">
-        <v>26</v>
+        <v>8140</v>
       </c>
       <c r="E26">
-        <v>12897</v>
+        <v>8732</v>
       </c>
       <c r="F26">
-        <v>569</v>
+        <v>3974</v>
       </c>
       <c r="G26">
-        <v>126</v>
+        <v>58033</v>
       </c>
       <c r="H26">
-        <v>194</v>
+        <v>1605</v>
       </c>
       <c r="I26" s="12">
-        <v>18</v>
+        <v>414</v>
       </c>
       <c r="J26" s="14">
-        <v>2</v>
+        <v>573</v>
       </c>
       <c r="K26">
         <f>(I26/C26)*10000</f>
-        <v>13.032145960034754</v>
+        <v>51.438795288504544</v>
       </c>
       <c r="L26">
         <f>(J26/C26)*10000</f>
-        <v>1.4480162177816391</v>
+        <v>71.194274638437463</v>
       </c>
       <c r="M26" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="27" spans="1:13">
       <c r="A27">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C27">
-        <v>17841</v>
+        <v>18238</v>
       </c>
       <c r="D27">
-        <v>973</v>
+        <v>2313</v>
       </c>
       <c r="E27">
-        <v>12821</v>
+        <v>13247</v>
       </c>
       <c r="F27">
-        <v>542</v>
+        <v>465</v>
       </c>
       <c r="G27">
-        <v>2942</v>
+        <v>1810</v>
       </c>
       <c r="H27">
-        <v>563</v>
+        <v>403</v>
       </c>
       <c r="I27" s="12">
-        <v>36</v>
+        <v>90</v>
       </c>
       <c r="J27" s="12">
-        <v>444</v>
+        <v>81</v>
       </c>
       <c r="K27">
         <f>(I27/C27)*10000</f>
-        <v>20.178241129981505</v>
+        <v>49.347516175019187</v>
       </c>
       <c r="L27">
         <f>(J27/C27)*10000</f>
-        <v>248.86497393643853</v>
+        <v>44.412764557517271</v>
       </c>
       <c r="M27" t="s">
         <v>173</v>
@@ -5875,42 +5875,42 @@
     </row>
     <row r="28" spans="1:13">
       <c r="A28">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="B28" t="s">
-        <v>42</v>
+        <v>78</v>
       </c>
       <c r="C28">
-        <v>11717</v>
+        <v>26493</v>
       </c>
       <c r="D28">
         <v>12</v>
       </c>
       <c r="E28">
-        <v>11370</v>
+        <v>25793</v>
       </c>
       <c r="F28">
-        <v>104</v>
+        <v>258</v>
       </c>
       <c r="G28">
-        <v>87</v>
+        <v>121</v>
       </c>
       <c r="H28">
-        <v>144</v>
+        <v>309</v>
       </c>
       <c r="I28" s="12">
-        <v>205</v>
+        <v>130</v>
       </c>
       <c r="J28" s="14">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="K28">
         <f>(I28/C28)*10000</f>
-        <v>174.95946061278485</v>
+        <v>49.069565545615824</v>
       </c>
       <c r="L28">
         <f>(J28/C28)*10000</f>
-        <v>0.85346078347699927</v>
+        <v>6.4167893405805305</v>
       </c>
       <c r="M28" t="s">
         <v>173</v>
@@ -5918,341 +5918,343 @@
     </row>
     <row r="29" spans="1:13">
       <c r="A29">
+        <v>75</v>
+      </c>
+      <c r="B29" t="s">
+        <v>80</v>
+      </c>
+      <c r="C29">
+        <v>22544</v>
+      </c>
+      <c r="D29">
+        <v>92</v>
+      </c>
+      <c r="E29">
+        <v>15039</v>
+      </c>
+      <c r="F29">
+        <v>619</v>
+      </c>
+      <c r="G29">
+        <v>6473</v>
+      </c>
+      <c r="H29">
+        <v>321</v>
+      </c>
+      <c r="I29" s="12">
+        <v>103</v>
+      </c>
+      <c r="J29" s="12">
         <v>3</v>
-      </c>
-      <c r="B29" t="s">
-        <v>30</v>
-      </c>
-      <c r="C29">
-        <v>56362</v>
-      </c>
-      <c r="D29">
-        <v>6414</v>
-      </c>
-      <c r="E29">
-        <v>11275</v>
-      </c>
-      <c r="F29">
-        <v>8009</v>
-      </c>
-      <c r="G29">
-        <v>29098</v>
-      </c>
-      <c r="H29">
-        <v>1566</v>
-      </c>
-      <c r="I29" s="12">
-        <v>517</v>
-      </c>
-      <c r="J29" s="12">
-        <v>6</v>
       </c>
       <c r="K29">
         <f>(I29/C29)*10000</f>
-        <v>91.728469536212344</v>
+        <v>45.688431511710434</v>
       </c>
       <c r="L29">
         <f>(J29/C29)*10000</f>
-        <v>1.064547035236507</v>
+        <v>1.3307310149041873</v>
       </c>
       <c r="M29" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="30" spans="1:13">
       <c r="A30">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C30">
-        <v>79288</v>
+        <v>54881</v>
       </c>
       <c r="D30">
-        <v>113</v>
+        <v>8022</v>
       </c>
       <c r="E30">
-        <v>10374</v>
+        <v>17303</v>
       </c>
       <c r="F30">
-        <v>65457</v>
+        <v>5048</v>
       </c>
       <c r="G30">
-        <v>3056</v>
+        <v>23042</v>
       </c>
       <c r="H30">
-        <v>288</v>
+        <v>1466</v>
       </c>
       <c r="I30" s="12">
-        <v>760</v>
+        <v>247</v>
       </c>
       <c r="J30" s="14">
-        <v>17</v>
+        <v>727</v>
       </c>
       <c r="K30">
         <f>(I30/C30)*10000</f>
-        <v>95.853092523458784</v>
+        <v>45.006468541025122</v>
       </c>
       <c r="L30">
         <f>(J30/C30)*10000</f>
-        <v>2.1440823327615779</v>
+        <v>132.46843169767314</v>
       </c>
       <c r="M30" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="31" spans="1:13">
       <c r="A31">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="B31" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="C31">
-        <v>10185</v>
+        <v>82236</v>
       </c>
       <c r="D31">
-        <v>19</v>
+        <v>3106</v>
       </c>
       <c r="E31">
-        <v>9751</v>
+        <v>6404</v>
       </c>
       <c r="F31">
-        <v>153</v>
+        <v>23901</v>
       </c>
       <c r="G31">
-        <v>81</v>
+        <v>47051</v>
       </c>
       <c r="H31">
-        <v>181</v>
+        <v>1774</v>
       </c>
       <c r="I31" s="12">
-        <v>19</v>
-      </c>
-      <c r="J31" s="15"/>
+        <v>331</v>
+      </c>
+      <c r="J31" s="14">
+        <v>42</v>
+      </c>
       <c r="K31">
         <f>(I31/C31)*10000</f>
-        <v>18.654884634266079</v>
+        <v>40.25001216012452</v>
       </c>
       <c r="L31">
         <f>(J31/C31)*10000</f>
-        <v>0</v>
+        <v>5.1072522982635347</v>
       </c>
       <c r="M31" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="32" spans="1:13">
       <c r="A32">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="B32" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="C32">
-        <v>15109</v>
+        <v>78743</v>
       </c>
       <c r="D32">
-        <v>18</v>
+        <v>1537</v>
       </c>
       <c r="E32">
-        <v>9354</v>
+        <v>2493</v>
       </c>
       <c r="F32">
-        <v>4809</v>
+        <v>62101</v>
       </c>
       <c r="G32">
-        <v>725</v>
+        <v>11959</v>
       </c>
       <c r="H32">
-        <v>203</v>
+        <v>653</v>
       </c>
       <c r="I32" s="12">
-        <v>36</v>
+        <v>293</v>
       </c>
       <c r="J32" s="12">
-        <v>168</v>
+        <v>3</v>
       </c>
       <c r="K32">
         <f>(I32/C32)*10000</f>
-        <v>23.826858164008208</v>
+        <v>37.209656731392002</v>
       </c>
       <c r="L32">
         <f>(J32/C32)*10000</f>
-        <v>111.19200476537164</v>
+        <v>0.38098624639650508</v>
       </c>
       <c r="M32" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="33" spans="1:13">
       <c r="A33">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>83</v>
+        <v>32</v>
       </c>
       <c r="C33">
-        <v>80484</v>
+        <v>35769</v>
       </c>
       <c r="D33">
-        <v>8140</v>
+        <v>371</v>
       </c>
       <c r="E33">
-        <v>8732</v>
+        <v>1108</v>
       </c>
       <c r="F33">
-        <v>3974</v>
+        <v>29486</v>
       </c>
       <c r="G33">
-        <v>58033</v>
+        <v>4447</v>
       </c>
       <c r="H33">
-        <v>1605</v>
+        <v>357</v>
       </c>
       <c r="I33" s="12">
-        <v>414</v>
+        <v>125</v>
       </c>
       <c r="J33" s="14">
-        <v>573</v>
+        <v>265</v>
       </c>
       <c r="K33">
         <f>(I33/C33)*10000</f>
-        <v>51.438795288504544</v>
+        <v>34.946462020185074</v>
       </c>
       <c r="L33">
         <f>(J33/C33)*10000</f>
-        <v>71.194274638437463</v>
+        <v>74.086499482792362</v>
       </c>
       <c r="M33" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="34" spans="1:13">
       <c r="A34">
-        <v>77</v>
+        <v>36</v>
       </c>
       <c r="B34" t="s">
-        <v>82</v>
+        <v>37</v>
       </c>
       <c r="C34">
-        <v>56521</v>
+        <v>5918</v>
       </c>
       <c r="D34">
-        <v>6582</v>
+        <v>35</v>
       </c>
       <c r="E34">
-        <v>8104</v>
+        <v>5567</v>
       </c>
       <c r="F34">
-        <v>9318</v>
+        <v>87</v>
       </c>
       <c r="G34">
-        <v>30889</v>
+        <v>122</v>
       </c>
       <c r="H34">
-        <v>1628</v>
+        <v>107</v>
       </c>
       <c r="I34" s="12">
-        <v>447</v>
+        <v>20</v>
       </c>
       <c r="J34" s="14">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="K34">
         <f>(I34/C34)*10000</f>
-        <v>79.08564958157146</v>
+        <v>33.795201081446436</v>
       </c>
       <c r="L34">
         <f>(J34/C34)*10000</f>
-        <v>7.7847171847631857</v>
+        <v>99.69584319026697</v>
       </c>
       <c r="M34" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="35" spans="1:13">
       <c r="A35">
+        <v>15</v>
+      </c>
+      <c r="B35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35">
+        <v>64124</v>
+      </c>
+      <c r="D35">
+        <v>2972</v>
+      </c>
+      <c r="E35">
+        <v>856</v>
+      </c>
+      <c r="F35">
+        <v>24861</v>
+      </c>
+      <c r="G35">
+        <v>34329</v>
+      </c>
+      <c r="H35">
+        <v>1106</v>
+      </c>
+      <c r="I35" s="12">
+        <v>208</v>
+      </c>
+      <c r="J35" s="14">
         <v>2</v>
-      </c>
-      <c r="B35" t="s">
-        <v>19</v>
-      </c>
-      <c r="C35">
-        <v>71942</v>
-      </c>
-      <c r="D35">
-        <v>16184</v>
-      </c>
-      <c r="E35">
-        <v>8015</v>
-      </c>
-      <c r="F35">
-        <v>14701</v>
-      </c>
-      <c r="G35">
-        <v>30706</v>
-      </c>
-      <c r="H35">
-        <v>2336</v>
-      </c>
-      <c r="I35" s="12">
-        <v>121</v>
-      </c>
-      <c r="J35" s="14">
-        <v>270</v>
       </c>
       <c r="K35">
         <f>(I35/C35)*10000</f>
-        <v>16.819104278446527</v>
+        <v>32.437153016031438</v>
       </c>
       <c r="L35">
         <f>(J35/C35)*10000</f>
-        <v>37.530232687442663</v>
+        <v>0.31189570207722539</v>
       </c>
       <c r="M35" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="36" spans="1:13">
       <c r="A36">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B36" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C36">
-        <v>25681</v>
+        <v>21390</v>
       </c>
       <c r="D36">
-        <v>3185</v>
+        <v>3307</v>
       </c>
       <c r="E36">
-        <v>7815</v>
+        <v>6015</v>
       </c>
       <c r="F36">
-        <v>1626</v>
+        <v>1202</v>
       </c>
       <c r="G36">
-        <v>11992</v>
+        <v>10281</v>
       </c>
       <c r="H36">
-        <v>1063</v>
+        <v>585</v>
       </c>
       <c r="I36" s="12">
-        <v>16</v>
+        <v>63</v>
       </c>
       <c r="J36" s="14">
-        <v>71</v>
+        <v>284</v>
       </c>
       <c r="K36">
         <f>(I36/C36)*10000</f>
-        <v>6.2302869825941363</v>
+        <v>29.453015427769987</v>
       </c>
       <c r="L36">
         <f>(J36/C36)*10000</f>
-        <v>27.646898485261477</v>
+        <v>132.77232351566153</v>
       </c>
       <c r="M36" t="s">
         <v>176</v>
@@ -6260,255 +6262,255 @@
     </row>
     <row r="37" spans="1:13">
       <c r="A37">
-        <v>72</v>
+        <v>22</v>
       </c>
       <c r="B37" t="s">
-        <v>77</v>
+        <v>22</v>
       </c>
       <c r="C37">
-        <v>20034</v>
+        <v>72791</v>
       </c>
       <c r="D37">
-        <v>112</v>
+        <v>1828</v>
       </c>
       <c r="E37">
-        <v>6838</v>
+        <v>3900</v>
       </c>
       <c r="F37">
-        <v>915</v>
+        <v>37295</v>
       </c>
       <c r="G37">
-        <v>11785</v>
+        <v>28514</v>
       </c>
       <c r="H37">
-        <v>384</v>
+        <v>1254</v>
       </c>
       <c r="I37" s="12">
-        <v>17</v>
-      </c>
-      <c r="J37" s="15"/>
+        <v>210</v>
+      </c>
+      <c r="J37" s="14">
+        <v>26</v>
+      </c>
       <c r="K37">
         <f>(I37/C37)*10000</f>
-        <v>8.4855745233103725</v>
+        <v>28.849720432471045</v>
       </c>
       <c r="L37">
         <f>(J37/C37)*10000</f>
-        <v>0</v>
+        <v>3.5718701487821294</v>
       </c>
       <c r="M37" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="38" spans="1:13">
       <c r="A38">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="C38">
-        <v>82236</v>
+        <v>2876</v>
       </c>
       <c r="D38">
-        <v>3106</v>
+        <v>7</v>
       </c>
       <c r="E38">
-        <v>6404</v>
+        <v>2651</v>
       </c>
       <c r="F38">
-        <v>23901</v>
+        <v>132</v>
       </c>
       <c r="G38">
-        <v>47051</v>
+        <v>47</v>
       </c>
       <c r="H38">
-        <v>1774</v>
+        <v>39</v>
       </c>
       <c r="I38" s="12">
-        <v>331</v>
-      </c>
-      <c r="J38" s="14">
-        <v>42</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="J38" s="15"/>
       <c r="K38">
         <f>(I38/C38)*10000</f>
-        <v>40.25001216012452</v>
+        <v>27.816411682892905</v>
       </c>
       <c r="L38">
         <f>(J38/C38)*10000</f>
-        <v>5.1072522982635347</v>
+        <v>0</v>
       </c>
       <c r="M38" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="39" spans="1:13">
       <c r="A39">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="B39" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="C39">
-        <v>6482</v>
+        <v>25010</v>
       </c>
       <c r="D39">
-        <v>2</v>
+        <v>294</v>
       </c>
       <c r="E39">
-        <v>6251</v>
+        <v>757</v>
       </c>
       <c r="F39">
-        <v>132</v>
+        <v>21860</v>
       </c>
       <c r="G39">
-        <v>32</v>
+        <v>1913</v>
       </c>
       <c r="H39">
-        <v>65</v>
+        <v>186</v>
       </c>
       <c r="I39" s="12">
-        <v>3</v>
+        <v>67</v>
       </c>
       <c r="J39" s="14">
-        <v>99</v>
+        <v>11</v>
       </c>
       <c r="K39">
         <f>(I39/C39)*10000</f>
-        <v>4.6282011724776302</v>
+        <v>26.789284286285486</v>
       </c>
       <c r="L39">
         <f>(J39/C39)*10000</f>
-        <v>152.73063869176181</v>
+        <v>4.3982407037185123</v>
       </c>
       <c r="M39" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="40" spans="1:13">
       <c r="A40">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B40" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="C40">
-        <v>7325</v>
+        <v>31977</v>
       </c>
       <c r="D40">
-        <v>5</v>
+        <v>11038</v>
       </c>
       <c r="E40">
-        <v>6122</v>
+        <v>672</v>
       </c>
       <c r="F40">
-        <v>571</v>
+        <v>8627</v>
       </c>
       <c r="G40">
-        <v>522</v>
+        <v>11225</v>
       </c>
       <c r="H40">
-        <v>105</v>
+        <v>415</v>
       </c>
       <c r="I40" s="12">
-        <v>18</v>
+        <v>81</v>
       </c>
       <c r="J40" s="14">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="K40">
         <f>(I40/C40)*10000</f>
-        <v>24.573378839590443</v>
+        <v>25.330706445257526</v>
       </c>
       <c r="L40">
         <f>(J40/C40)*10000</f>
-        <v>1.3651877133105803</v>
+        <v>8.756293586014948</v>
       </c>
       <c r="M40" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="41" spans="1:13">
       <c r="A41">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="B41" t="s">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="C41">
-        <v>21390</v>
+        <v>45368</v>
       </c>
       <c r="D41">
-        <v>3307</v>
+        <v>2252</v>
       </c>
       <c r="E41">
-        <v>6015</v>
+        <v>542</v>
       </c>
       <c r="F41">
-        <v>1202</v>
+        <v>38693</v>
       </c>
       <c r="G41">
-        <v>10281</v>
+        <v>3682</v>
       </c>
       <c r="H41">
-        <v>585</v>
+        <v>199</v>
       </c>
       <c r="I41" s="12">
-        <v>63</v>
+        <v>113</v>
       </c>
       <c r="J41" s="14">
-        <v>284</v>
+        <v>1</v>
       </c>
       <c r="K41">
         <f>(I41/C41)*10000</f>
-        <v>29.453015427769987</v>
+        <v>24.907423734791042</v>
       </c>
       <c r="L41">
         <f>(J41/C41)*10000</f>
-        <v>132.77232351566153</v>
+        <v>0.22041967906894727</v>
       </c>
       <c r="M41" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="42" spans="1:13">
       <c r="A42">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="B42" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="C42">
-        <v>5918</v>
+        <v>7325</v>
       </c>
       <c r="D42">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="E42">
-        <v>5567</v>
+        <v>6122</v>
       </c>
       <c r="F42">
-        <v>87</v>
+        <v>571</v>
       </c>
       <c r="G42">
-        <v>122</v>
+        <v>522</v>
       </c>
       <c r="H42">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I42" s="12">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J42" s="14">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="K42">
         <f>(I42/C42)*10000</f>
-        <v>33.795201081446436</v>
+        <v>24.573378839590443</v>
       </c>
       <c r="L42">
         <f>(J42/C42)*10000</f>
-        <v>99.69584319026697</v>
+        <v>1.3651877133105803</v>
       </c>
       <c r="M42" t="s">
         <v>173</v>
@@ -6516,85 +6518,85 @@
     </row>
     <row r="43" spans="1:13">
       <c r="A43">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="B43" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="C43">
-        <v>72791</v>
+        <v>15109</v>
       </c>
       <c r="D43">
-        <v>1828</v>
+        <v>18</v>
       </c>
       <c r="E43">
-        <v>3900</v>
+        <v>9354</v>
       </c>
       <c r="F43">
-        <v>37295</v>
+        <v>4809</v>
       </c>
       <c r="G43">
-        <v>28514</v>
+        <v>725</v>
       </c>
       <c r="H43">
-        <v>1254</v>
+        <v>203</v>
       </c>
       <c r="I43" s="12">
-        <v>210</v>
+        <v>36</v>
       </c>
       <c r="J43" s="14">
-        <v>26</v>
+        <v>168</v>
       </c>
       <c r="K43">
         <f>(I43/C43)*10000</f>
-        <v>28.849720432471045</v>
+        <v>23.826858164008208</v>
       </c>
       <c r="L43">
         <f>(J43/C43)*10000</f>
-        <v>3.5718701487821294</v>
+        <v>111.19200476537164</v>
       </c>
       <c r="M43" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="44" spans="1:13">
       <c r="A44">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B44" t="s">
-        <v>63</v>
+        <v>10</v>
       </c>
       <c r="C44">
-        <v>94368</v>
+        <v>25448</v>
       </c>
       <c r="D44">
-        <v>5653</v>
+        <v>2256</v>
       </c>
       <c r="E44">
-        <v>3651</v>
+        <v>265</v>
       </c>
       <c r="F44">
-        <v>7198</v>
+        <v>4927</v>
       </c>
       <c r="G44">
-        <v>75845</v>
+        <v>17475</v>
       </c>
       <c r="H44">
-        <v>2021</v>
+        <v>525</v>
       </c>
       <c r="I44" s="12">
-        <v>142</v>
+        <v>59</v>
       </c>
       <c r="J44" s="14">
-        <v>343</v>
+        <v>3</v>
       </c>
       <c r="K44">
         <f>(I44/C44)*10000</f>
-        <v>15.047473719905053</v>
+        <v>23.184533165671173</v>
       </c>
       <c r="L44">
         <f>(J44/C44)*10000</f>
-        <v>36.347066802305868</v>
+        <v>1.178874567745992</v>
       </c>
       <c r="M44" t="s">
         <v>175</v>
@@ -6602,83 +6604,85 @@
     </row>
     <row r="45" spans="1:13">
       <c r="A45">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="B45" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="C45">
-        <v>29283</v>
+        <v>15612</v>
       </c>
       <c r="D45">
-        <v>4658</v>
+        <v>2445</v>
       </c>
       <c r="E45">
-        <v>3361</v>
+        <v>234</v>
       </c>
       <c r="F45">
-        <v>2010</v>
+        <v>10111</v>
       </c>
       <c r="G45">
-        <v>18359</v>
+        <v>2667</v>
       </c>
       <c r="H45">
-        <v>895</v>
+        <v>155</v>
       </c>
       <c r="I45" s="12">
-        <v>170</v>
+        <v>35</v>
       </c>
       <c r="J45" s="14">
-        <v>241</v>
+        <v>1</v>
       </c>
       <c r="K45">
         <f>(I45/C45)*10000</f>
-        <v>58.054161117371855</v>
+        <v>22.418652318729183</v>
       </c>
       <c r="L45">
         <f>(J45/C45)*10000</f>
-        <v>82.300310760509504</v>
+        <v>0.64053292339226231</v>
       </c>
       <c r="M45" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="46" spans="1:13">
       <c r="A46">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B46" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C46">
-        <v>2916</v>
+        <v>17841</v>
       </c>
       <c r="D46">
-        <v>0</v>
+        <v>973</v>
       </c>
       <c r="E46">
-        <v>2849</v>
+        <v>12821</v>
       </c>
       <c r="F46">
-        <v>20</v>
+        <v>542</v>
       </c>
       <c r="G46">
-        <v>19</v>
+        <v>2942</v>
       </c>
       <c r="H46">
-        <v>28</v>
+        <v>563</v>
       </c>
       <c r="I46" s="12">
-        <v>2</v>
-      </c>
-      <c r="J46" s="16"/>
+        <v>36</v>
+      </c>
+      <c r="J46" s="12">
+        <v>444</v>
+      </c>
       <c r="K46">
         <f>(I46/C46)*10000</f>
-        <v>6.8587105624142657</v>
+        <v>20.178241129981505</v>
       </c>
       <c r="L46">
         <f>(J46/C46)*10000</f>
-        <v>0</v>
+        <v>248.86497393643853</v>
       </c>
       <c r="M46" t="s">
         <v>173</v>
@@ -6686,79 +6690,79 @@
     </row>
     <row r="47" spans="1:13">
       <c r="A47">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="B47" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C47">
-        <v>64116</v>
+        <v>39894</v>
       </c>
       <c r="D47">
-        <v>3296</v>
+        <v>121</v>
       </c>
       <c r="E47">
-        <v>2753</v>
+        <v>2161</v>
       </c>
       <c r="F47">
-        <v>3571</v>
+        <v>35589</v>
       </c>
       <c r="G47">
-        <v>53138</v>
+        <v>1892</v>
       </c>
       <c r="H47">
-        <v>1358</v>
+        <v>131</v>
       </c>
       <c r="I47" s="12">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="J47" s="14">
-        <v>267</v>
+        <v>1</v>
       </c>
       <c r="K47">
         <f>(I47/C47)*10000</f>
-        <v>15.440763615946098</v>
+        <v>20.05314082318143</v>
       </c>
       <c r="L47">
         <f>(J47/C47)*10000</f>
-        <v>41.64327157027887</v>
+        <v>0.2506642602897679</v>
       </c>
       <c r="M47" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="48" spans="1:13">
       <c r="A48">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B48" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="C48">
-        <v>2876</v>
+        <v>10185</v>
       </c>
       <c r="D48">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="E48">
-        <v>2651</v>
+        <v>9751</v>
       </c>
       <c r="F48">
-        <v>132</v>
+        <v>153</v>
       </c>
       <c r="G48">
-        <v>47</v>
+        <v>81</v>
       </c>
       <c r="H48">
-        <v>39</v>
+        <v>181</v>
       </c>
       <c r="I48" s="12">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="J48" s="16"/>
       <c r="K48">
         <f>(I48/C48)*10000</f>
-        <v>27.816411682892905</v>
+        <v>18.654884634266079</v>
       </c>
       <c r="L48">
         <f>(J48/C48)*10000</f>
@@ -6770,169 +6774,171 @@
     </row>
     <row r="49" spans="1:13">
       <c r="A49">
+        <v>2</v>
+      </c>
+      <c r="B49" t="s">
         <v>19</v>
       </c>
-      <c r="B49" t="s">
-        <v>18</v>
-      </c>
       <c r="C49">
-        <v>78743</v>
+        <v>71942</v>
       </c>
       <c r="D49">
-        <v>1537</v>
+        <v>16184</v>
       </c>
       <c r="E49">
-        <v>2493</v>
+        <v>8015</v>
       </c>
       <c r="F49">
-        <v>62101</v>
+        <v>14701</v>
       </c>
       <c r="G49">
-        <v>11959</v>
+        <v>30706</v>
       </c>
       <c r="H49">
-        <v>653</v>
+        <v>2336</v>
       </c>
       <c r="I49" s="12">
-        <v>293</v>
+        <v>121</v>
       </c>
       <c r="J49" s="14">
-        <v>3</v>
+        <v>270</v>
       </c>
       <c r="K49">
         <f>(I49/C49)*10000</f>
-        <v>37.209656731392002</v>
+        <v>16.819104278446527</v>
       </c>
       <c r="L49">
         <f>(J49/C49)*10000</f>
-        <v>0.38098624639650508</v>
+        <v>37.530232687442663</v>
       </c>
       <c r="M49" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="50" spans="1:13">
       <c r="A50">
-        <v>63</v>
+        <v>7</v>
       </c>
       <c r="B50" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="C50">
-        <v>39894</v>
+        <v>64116</v>
       </c>
       <c r="D50">
-        <v>121</v>
+        <v>3296</v>
       </c>
       <c r="E50">
-        <v>2161</v>
+        <v>2753</v>
       </c>
       <c r="F50">
-        <v>35589</v>
+        <v>3571</v>
       </c>
       <c r="G50">
-        <v>1892</v>
+        <v>53138</v>
       </c>
       <c r="H50">
-        <v>131</v>
+        <v>1358</v>
       </c>
       <c r="I50" s="12">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="J50" s="14">
-        <v>1</v>
+        <v>267</v>
       </c>
       <c r="K50">
         <f>(I50/C50)*10000</f>
-        <v>20.05314082318143</v>
+        <v>15.440763615946098</v>
       </c>
       <c r="L50">
         <f>(J50/C50)*10000</f>
-        <v>0.2506642602897679</v>
+        <v>41.64327157027887</v>
       </c>
       <c r="M50" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="51" spans="1:13">
       <c r="A51">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B51" t="s">
+        <v>41</v>
+      </c>
+      <c r="C51">
+        <v>39493</v>
+      </c>
+      <c r="D51">
+        <v>4399</v>
+      </c>
+      <c r="E51">
+        <v>1488</v>
+      </c>
+      <c r="F51">
+        <v>7562</v>
+      </c>
+      <c r="G51">
+        <v>24916</v>
+      </c>
+      <c r="H51">
+        <v>1128</v>
+      </c>
+      <c r="I51" s="12">
+        <v>60</v>
+      </c>
+      <c r="J51" s="14">
         <v>13</v>
-      </c>
-      <c r="C51">
-        <v>51542</v>
-      </c>
-      <c r="D51">
-        <v>7430</v>
-      </c>
-      <c r="E51">
-        <v>2076</v>
-      </c>
-      <c r="F51">
-        <v>25487</v>
-      </c>
-      <c r="G51">
-        <v>15054</v>
-      </c>
-      <c r="H51">
-        <v>1495</v>
-      </c>
-      <c r="I51" s="12">
-        <v>65</v>
-      </c>
-      <c r="J51" s="14">
-        <v>32</v>
       </c>
       <c r="K51">
         <f>(I51/C51)*10000</f>
-        <v>12.611074463544293</v>
+        <v>15.192565771149317</v>
       </c>
       <c r="L51">
         <f>(J51/C51)*10000</f>
-        <v>6.2085289666679602</v>
+        <v>3.2917225837490189</v>
       </c>
       <c r="M51" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="52" spans="1:13">
       <c r="A52">
-        <v>56</v>
+        <v>6</v>
       </c>
       <c r="B52" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C52">
-        <v>34513</v>
+        <v>94368</v>
       </c>
       <c r="D52">
-        <v>346</v>
+        <v>5653</v>
       </c>
       <c r="E52">
-        <v>2040</v>
+        <v>3651</v>
       </c>
       <c r="F52">
-        <v>13515</v>
+        <v>7198</v>
       </c>
       <c r="G52">
-        <v>18372</v>
+        <v>75845</v>
       </c>
       <c r="H52">
-        <v>240</v>
+        <v>2021</v>
       </c>
       <c r="I52" s="12">
-        <v>21</v>
-      </c>
-      <c r="J52" s="15"/>
+        <v>142</v>
+      </c>
+      <c r="J52" s="14">
+        <v>343</v>
+      </c>
       <c r="K52">
         <f>(I52/C52)*10000</f>
-        <v>6.0846637498913454</v>
+        <v>15.047473719905053</v>
       </c>
       <c r="L52">
         <f>(J52/C52)*10000</f>
-        <v>0</v>
+        <v>36.347066802305868</v>
       </c>
       <c r="M52" t="s">
         <v>175</v>
@@ -6940,341 +6946,341 @@
     </row>
     <row r="53" spans="1:13">
       <c r="A53">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="C53">
-        <v>53359</v>
+        <v>23042</v>
       </c>
       <c r="D53">
-        <v>3736</v>
+        <v>53</v>
       </c>
       <c r="E53">
-        <v>1736</v>
+        <v>777</v>
       </c>
       <c r="F53">
-        <v>24332</v>
+        <v>18076</v>
       </c>
       <c r="G53">
-        <v>22234</v>
+        <v>3969</v>
       </c>
       <c r="H53">
-        <v>1321</v>
+        <v>167</v>
       </c>
       <c r="I53" s="12">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="J53" s="14">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="K53">
         <f>(I53/C53)*10000</f>
-        <v>11.619408159823086</v>
+        <v>13.453693255793768</v>
       </c>
       <c r="L53">
         <f>(J53/C53)*10000</f>
-        <v>5.2474746528233283</v>
+        <v>1.7359604201024217</v>
       </c>
       <c r="M53" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="54" spans="1:13">
       <c r="A54">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B54" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="C54">
-        <v>39493</v>
+        <v>39262</v>
       </c>
       <c r="D54">
-        <v>4399</v>
+        <v>1194</v>
       </c>
       <c r="E54">
-        <v>1488</v>
+        <v>991</v>
       </c>
       <c r="F54">
-        <v>7562</v>
+        <v>25295</v>
       </c>
       <c r="G54">
-        <v>24916</v>
+        <v>11166</v>
       </c>
       <c r="H54">
-        <v>1128</v>
+        <v>616</v>
       </c>
       <c r="I54" s="12">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="J54" s="14">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="K54">
         <f>(I54/C54)*10000</f>
-        <v>15.192565771149317</v>
+        <v>13.244358412714584</v>
       </c>
       <c r="L54">
         <f>(J54/C54)*10000</f>
-        <v>3.2917225837490189</v>
+        <v>5.6033824053792474</v>
       </c>
       <c r="M54" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="55" spans="1:13">
       <c r="A55">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="B55" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C55">
-        <v>13391</v>
+        <v>13812</v>
       </c>
       <c r="D55">
-        <v>9721</v>
+        <v>26</v>
       </c>
       <c r="E55">
-        <v>1419</v>
+        <v>12897</v>
       </c>
       <c r="F55">
-        <v>464</v>
+        <v>569</v>
       </c>
       <c r="G55">
-        <v>1642</v>
+        <v>126</v>
       </c>
       <c r="H55">
-        <v>145</v>
+        <v>194</v>
       </c>
       <c r="I55" s="12">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J55" s="12">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="K55">
         <f>(I55/C55)*10000</f>
-        <v>11.948323500858786</v>
+        <v>13.032145960034754</v>
       </c>
       <c r="L55">
         <f>(J55/C55)*10000</f>
-        <v>9.7080128444477634</v>
+        <v>1.4480162177816391</v>
       </c>
       <c r="M55" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="56" spans="1:13">
       <c r="A56">
+        <v>14</v>
+      </c>
+      <c r="B56" t="s">
+        <v>13</v>
+      </c>
+      <c r="C56">
+        <v>51542</v>
+      </c>
+      <c r="D56">
+        <v>7430</v>
+      </c>
+      <c r="E56">
+        <v>2076</v>
+      </c>
+      <c r="F56">
+        <v>25487</v>
+      </c>
+      <c r="G56">
+        <v>15054</v>
+      </c>
+      <c r="H56">
+        <v>1495</v>
+      </c>
+      <c r="I56" s="12">
         <v>65</v>
       </c>
-      <c r="B56" t="s">
-        <v>69</v>
-      </c>
-      <c r="C56">
-        <v>33355</v>
-      </c>
-      <c r="D56">
-        <v>210</v>
-      </c>
-      <c r="E56">
-        <v>1390</v>
-      </c>
-      <c r="F56">
-        <v>26669</v>
-      </c>
-      <c r="G56">
-        <v>4924</v>
-      </c>
-      <c r="H56">
-        <v>162</v>
-      </c>
-      <c r="I56" s="12">
-        <v>26</v>
-      </c>
       <c r="J56" s="14">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="K56">
         <f>(I56/C56)*10000</f>
-        <v>7.7949332933593158</v>
+        <v>12.611074463544293</v>
       </c>
       <c r="L56">
         <f>(J56/C56)*10000</f>
-        <v>0.59961025333533202</v>
+        <v>6.2085289666679602</v>
       </c>
       <c r="M56" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="57" spans="1:13">
       <c r="A57">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B57" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C57">
-        <v>35769</v>
+        <v>13391</v>
       </c>
       <c r="D57">
-        <v>371</v>
+        <v>9721</v>
       </c>
       <c r="E57">
-        <v>1108</v>
+        <v>1419</v>
       </c>
       <c r="F57">
-        <v>29486</v>
+        <v>464</v>
       </c>
       <c r="G57">
-        <v>4447</v>
+        <v>1642</v>
       </c>
       <c r="H57">
-        <v>357</v>
+        <v>145</v>
       </c>
       <c r="I57" s="12">
-        <v>125</v>
+        <v>16</v>
       </c>
       <c r="J57" s="12">
-        <v>265</v>
+        <v>13</v>
       </c>
       <c r="K57">
         <f>(I57/C57)*10000</f>
-        <v>34.946462020185074</v>
+        <v>11.948323500858786</v>
       </c>
       <c r="L57">
         <f>(J57/C57)*10000</f>
-        <v>74.086499482792362</v>
+        <v>9.7080128444477634</v>
       </c>
       <c r="M57" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="58" spans="1:13">
       <c r="A58">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B58" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C58">
-        <v>39262</v>
+        <v>53359</v>
       </c>
       <c r="D58">
-        <v>1194</v>
+        <v>3736</v>
       </c>
       <c r="E58">
-        <v>991</v>
+        <v>1736</v>
       </c>
       <c r="F58">
-        <v>25295</v>
+        <v>24332</v>
       </c>
       <c r="G58">
-        <v>11166</v>
+        <v>22234</v>
       </c>
       <c r="H58">
-        <v>616</v>
+        <v>1321</v>
       </c>
       <c r="I58" s="12">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="J58" s="14">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="K58">
         <f>(I58/C58)*10000</f>
-        <v>13.244358412714584</v>
+        <v>11.619408159823086</v>
       </c>
       <c r="L58">
         <f>(J58/C58)*10000</f>
-        <v>5.6033824053792474</v>
+        <v>5.2474746528233283</v>
       </c>
       <c r="M58" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="59" spans="1:13">
       <c r="A59">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B59" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C59">
-        <v>19093</v>
+        <v>41081</v>
       </c>
       <c r="D59">
-        <v>126</v>
+        <v>276</v>
       </c>
       <c r="E59">
-        <v>987</v>
+        <v>18976</v>
       </c>
       <c r="F59">
-        <v>1382</v>
+        <v>15132</v>
       </c>
       <c r="G59">
-        <v>16413</v>
+        <v>6251</v>
       </c>
       <c r="H59">
-        <v>185</v>
+        <v>446</v>
       </c>
       <c r="I59" s="12">
-        <v>13</v>
-      </c>
-      <c r="J59" s="15"/>
+        <v>38</v>
+      </c>
+      <c r="J59" s="14">
+        <v>3</v>
+      </c>
       <c r="K59">
         <f>(I59/C59)*10000</f>
-        <v>6.808778086209605</v>
+        <v>9.2500182566149807</v>
       </c>
       <c r="L59">
         <f>(J59/C59)*10000</f>
-        <v>0</v>
+        <v>0.73026459920644582</v>
       </c>
       <c r="M59" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="60" spans="1:13">
       <c r="A60">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="B60" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
       <c r="C60">
-        <v>64124</v>
+        <v>20034</v>
       </c>
       <c r="D60">
-        <v>2972</v>
+        <v>112</v>
       </c>
       <c r="E60">
-        <v>856</v>
+        <v>6838</v>
       </c>
       <c r="F60">
-        <v>24861</v>
+        <v>915</v>
       </c>
       <c r="G60">
-        <v>34329</v>
+        <v>11785</v>
       </c>
       <c r="H60">
-        <v>1106</v>
+        <v>384</v>
       </c>
       <c r="I60" s="12">
-        <v>208</v>
-      </c>
-      <c r="J60" s="14">
-        <v>2</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="J60" s="15"/>
       <c r="K60">
         <f>(I60/C60)*10000</f>
-        <v>32.437153016031438</v>
+        <v>8.4855745233103725</v>
       </c>
       <c r="L60">
         <f>(J60/C60)*10000</f>
-        <v>0.31189570207722539</v>
+        <v>0</v>
       </c>
       <c r="M60" t="s">
         <v>175</v>
@@ -7282,88 +7288,86 @@
     </row>
     <row r="61" spans="1:13">
       <c r="A61">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="B61" t="s">
-        <v>55</v>
+        <v>12</v>
       </c>
       <c r="C61">
-        <v>23042</v>
+        <v>17931</v>
       </c>
       <c r="D61">
-        <v>53</v>
+        <v>4600</v>
       </c>
       <c r="E61">
-        <v>777</v>
+        <v>573</v>
       </c>
       <c r="F61">
-        <v>18076</v>
+        <v>3224</v>
       </c>
       <c r="G61">
-        <v>3969</v>
+        <v>8847</v>
       </c>
       <c r="H61">
-        <v>167</v>
+        <v>687</v>
       </c>
       <c r="I61" s="12">
-        <v>31</v>
-      </c>
-      <c r="J61" s="14">
-        <v>4</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="J61" s="15"/>
       <c r="K61">
         <f>(I61/C61)*10000</f>
-        <v>13.453693255793768</v>
+        <v>8.365400702693659</v>
       </c>
       <c r="L61">
         <f>(J61/C61)*10000</f>
-        <v>1.7359604201024217</v>
+        <v>0</v>
       </c>
       <c r="M61" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="62" spans="1:13">
       <c r="A62">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B62" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C62">
-        <v>25010</v>
+        <v>41932</v>
       </c>
       <c r="D62">
-        <v>294</v>
+        <v>1587</v>
       </c>
       <c r="E62">
-        <v>757</v>
+        <v>308</v>
       </c>
       <c r="F62">
-        <v>21860</v>
+        <v>9997</v>
       </c>
       <c r="G62">
-        <v>1913</v>
+        <v>29512</v>
       </c>
       <c r="H62">
-        <v>186</v>
+        <v>528</v>
       </c>
       <c r="I62" s="12">
-        <v>67</v>
+        <v>35</v>
       </c>
       <c r="J62" s="14">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="K62">
         <f>(I62/C62)*10000</f>
-        <v>26.789284286285486</v>
+        <v>8.3468472765429738</v>
       </c>
       <c r="L62">
         <f>(J62/C62)*10000</f>
-        <v>4.3982407037185123</v>
+        <v>0.23848135075837071</v>
       </c>
       <c r="M62" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="63" spans="1:13">
@@ -7411,201 +7415,204 @@
     </row>
     <row r="64" spans="1:13">
       <c r="A64">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B64" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C64">
-        <v>31977</v>
+        <v>33355</v>
       </c>
       <c r="D64">
-        <v>11038</v>
+        <v>210</v>
       </c>
       <c r="E64">
-        <v>672</v>
+        <v>1390</v>
       </c>
       <c r="F64">
-        <v>8627</v>
+        <v>26669</v>
       </c>
       <c r="G64">
-        <v>11225</v>
+        <v>4924</v>
       </c>
       <c r="H64">
-        <v>415</v>
+        <v>162</v>
       </c>
       <c r="I64" s="12">
-        <v>81</v>
+        <v>26</v>
       </c>
       <c r="J64" s="14">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="K64">
         <f>(I64/C64)*10000</f>
-        <v>25.330706445257526</v>
+        <v>7.7949332933593158</v>
       </c>
       <c r="L64">
         <f>(J64/C64)*10000</f>
-        <v>8.756293586014948</v>
+        <v>0.59961025333533202</v>
       </c>
       <c r="M64" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="65" spans="1:13">
       <c r="A65">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="B65" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="C65">
-        <v>13426</v>
+        <v>2916</v>
       </c>
       <c r="D65">
-        <v>377</v>
+        <v>0</v>
       </c>
       <c r="E65">
-        <v>598</v>
+        <v>2849</v>
       </c>
       <c r="F65">
-        <v>7248</v>
+        <v>20</v>
       </c>
       <c r="G65">
-        <v>5041</v>
+        <v>19</v>
       </c>
       <c r="H65">
-        <v>162</v>
+        <v>28</v>
+      </c>
+      <c r="I65" s="12">
+        <v>2</v>
       </c>
       <c r="J65" s="15"/>
       <c r="K65">
         <f>(I65/C65)*10000</f>
-        <v>0</v>
+        <v>6.8587105624142657</v>
       </c>
       <c r="L65">
         <f>(J65/C65)*10000</f>
         <v>0</v>
       </c>
       <c r="M65" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="66" spans="1:13">
       <c r="A66">
+        <v>74</v>
+      </c>
+      <c r="B66" t="s">
+        <v>79</v>
+      </c>
+      <c r="C66">
+        <v>19093</v>
+      </c>
+      <c r="D66">
+        <v>126</v>
+      </c>
+      <c r="E66">
+        <v>987</v>
+      </c>
+      <c r="F66">
+        <v>1382</v>
+      </c>
+      <c r="G66">
+        <v>16413</v>
+      </c>
+      <c r="H66">
+        <v>185</v>
+      </c>
+      <c r="I66" s="12">
         <v>13</v>
-      </c>
-      <c r="B66" t="s">
-        <v>12</v>
-      </c>
-      <c r="C66">
-        <v>17931</v>
-      </c>
-      <c r="D66">
-        <v>4600</v>
-      </c>
-      <c r="E66">
-        <v>573</v>
-      </c>
-      <c r="F66">
-        <v>3224</v>
-      </c>
-      <c r="G66">
-        <v>8847</v>
-      </c>
-      <c r="H66">
-        <v>687</v>
-      </c>
-      <c r="I66" s="12">
-        <v>15</v>
       </c>
       <c r="J66" s="15"/>
       <c r="K66">
         <f>(I66/C66)*10000</f>
-        <v>8.365400702693659</v>
+        <v>6.808778086209605</v>
       </c>
       <c r="L66">
         <f>(J66/C66)*10000</f>
         <v>0</v>
       </c>
       <c r="M66" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="67" spans="1:13">
       <c r="A67">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="B67" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="C67">
-        <v>45368</v>
+        <v>25681</v>
       </c>
       <c r="D67">
-        <v>2252</v>
+        <v>3185</v>
       </c>
       <c r="E67">
-        <v>542</v>
+        <v>7815</v>
       </c>
       <c r="F67">
-        <v>38693</v>
+        <v>1626</v>
       </c>
       <c r="G67">
-        <v>3682</v>
+        <v>11992</v>
       </c>
       <c r="H67">
-        <v>199</v>
+        <v>1063</v>
       </c>
       <c r="I67" s="12">
-        <v>113</v>
+        <v>16</v>
       </c>
       <c r="J67" s="14">
-        <v>1</v>
+        <v>71</v>
       </c>
       <c r="K67">
         <f>(I67/C67)*10000</f>
-        <v>24.907423734791042</v>
+        <v>6.2302869825941363</v>
       </c>
       <c r="L67">
         <f>(J67/C67)*10000</f>
-        <v>0.22041967906894727</v>
+        <v>27.646898485261477</v>
       </c>
       <c r="M67" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="68" spans="1:13">
       <c r="A68">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="B68" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="C68">
-        <v>12756</v>
+        <v>34513</v>
       </c>
       <c r="D68">
-        <v>1058</v>
+        <v>346</v>
       </c>
       <c r="E68">
-        <v>403</v>
+        <v>2040</v>
       </c>
       <c r="F68">
-        <v>1212</v>
+        <v>13515</v>
       </c>
       <c r="G68">
-        <v>9845</v>
+        <v>18372</v>
       </c>
       <c r="H68">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="I68" s="12">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="J68" s="15"/>
       <c r="K68">
         <f>(I68/C68)*10000</f>
-        <v>0.7839448102853559</v>
+        <v>6.0846637498913454</v>
       </c>
       <c r="L68">
         <f>(J68/C68)*10000</f>
@@ -7617,255 +7624,253 @@
     </row>
     <row r="69" spans="1:13">
       <c r="A69">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="B69" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="C69">
-        <v>9426</v>
+        <v>23139</v>
       </c>
       <c r="D69">
-        <v>48</v>
+        <v>212</v>
       </c>
       <c r="E69">
-        <v>364</v>
+        <v>282</v>
       </c>
       <c r="F69">
-        <v>4671</v>
+        <v>10484</v>
       </c>
       <c r="G69">
-        <v>4235</v>
+        <v>11921</v>
       </c>
       <c r="H69">
-        <v>108</v>
+        <v>240</v>
       </c>
       <c r="I69" s="12">
-        <v>5</v>
-      </c>
-      <c r="J69" s="15"/>
+        <v>13</v>
+      </c>
+      <c r="J69" s="14">
+        <v>1</v>
+      </c>
       <c r="K69">
         <f>(I69/C69)*10000</f>
-        <v>5.3044769785699133</v>
+        <v>5.6182203206707282</v>
       </c>
       <c r="L69">
         <f>(J69/C69)*10000</f>
-        <v>0</v>
+        <v>0.43217079389774843</v>
       </c>
       <c r="M69" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="70" spans="1:13">
       <c r="A70">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="B70" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="C70">
-        <v>41932</v>
+        <v>9426</v>
       </c>
       <c r="D70">
-        <v>1587</v>
+        <v>48</v>
       </c>
       <c r="E70">
-        <v>308</v>
+        <v>364</v>
       </c>
       <c r="F70">
-        <v>9997</v>
+        <v>4671</v>
       </c>
       <c r="G70">
-        <v>29512</v>
+        <v>4235</v>
       </c>
       <c r="H70">
-        <v>528</v>
+        <v>108</v>
       </c>
       <c r="I70" s="12">
-        <v>35</v>
-      </c>
-      <c r="J70" s="14">
-        <v>1</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="J70" s="15"/>
       <c r="K70">
         <f>(I70/C70)*10000</f>
-        <v>8.3468472765429738</v>
+        <v>5.3044769785699133</v>
       </c>
       <c r="L70">
         <f>(J70/C70)*10000</f>
-        <v>0.23848135075837071</v>
+        <v>0</v>
       </c>
       <c r="M70" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="71" spans="1:13">
       <c r="A71">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B71" t="s">
-        <v>68</v>
+        <v>167</v>
       </c>
       <c r="C71">
-        <v>23139</v>
+        <v>13393</v>
       </c>
       <c r="D71">
-        <v>212</v>
+        <v>138</v>
       </c>
       <c r="E71">
-        <v>282</v>
+        <v>130</v>
       </c>
       <c r="F71">
-        <v>10484</v>
+        <v>10182</v>
       </c>
       <c r="G71">
-        <v>11921</v>
+        <v>2874</v>
       </c>
       <c r="H71">
-        <v>240</v>
+        <v>69</v>
       </c>
       <c r="I71" s="12">
-        <v>13</v>
-      </c>
-      <c r="J71" s="14">
-        <v>1</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="J71" s="15"/>
       <c r="K71">
         <f>(I71/C71)*10000</f>
-        <v>5.6182203206707282</v>
+        <v>5.2266109161502277</v>
       </c>
       <c r="L71">
         <f>(J71/C71)*10000</f>
-        <v>0.43217079389774843</v>
+        <v>0</v>
       </c>
       <c r="M71" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="72" spans="1:13">
       <c r="A72">
-        <v>11</v>
+        <v>54</v>
       </c>
       <c r="B72" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
       <c r="C72">
-        <v>25448</v>
+        <v>6482</v>
       </c>
       <c r="D72">
-        <v>2256</v>
+        <v>2</v>
       </c>
       <c r="E72">
-        <v>265</v>
+        <v>6251</v>
       </c>
       <c r="F72">
-        <v>4927</v>
+        <v>132</v>
       </c>
       <c r="G72">
-        <v>17475</v>
+        <v>32</v>
       </c>
       <c r="H72">
-        <v>525</v>
+        <v>65</v>
       </c>
       <c r="I72" s="12">
-        <v>59</v>
+        <v>3</v>
       </c>
       <c r="J72" s="14">
-        <v>3</v>
+        <v>99</v>
       </c>
       <c r="K72">
         <f>(I72/C72)*10000</f>
-        <v>23.184533165671173</v>
+        <v>4.6282011724776302</v>
       </c>
       <c r="L72">
         <f>(J72/C72)*10000</f>
-        <v>1.178874567745992</v>
+        <v>152.73063869176181</v>
       </c>
       <c r="M72" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="73" spans="1:13">
       <c r="A73">
-        <v>62</v>
+        <v>10</v>
       </c>
       <c r="B73" t="s">
-        <v>66</v>
+        <v>9</v>
       </c>
       <c r="C73">
-        <v>18109</v>
+        <v>37023</v>
       </c>
       <c r="D73">
-        <v>222</v>
+        <v>1696</v>
       </c>
       <c r="E73">
-        <v>255</v>
+        <v>164</v>
       </c>
       <c r="F73">
-        <v>14314</v>
+        <v>4442</v>
       </c>
       <c r="G73">
-        <v>3250</v>
+        <v>30157</v>
       </c>
       <c r="H73">
-        <v>68</v>
+        <v>564</v>
       </c>
       <c r="I73" s="12">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="J73" s="14">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="K73">
         <f>(I73/C73)*10000</f>
-        <v>2.7610580374399469</v>
+        <v>3.2412284255732922</v>
       </c>
       <c r="L73">
         <f>(J73/C73)*10000</f>
-        <v>11.596443757247776</v>
+        <v>1.0804094751910973</v>
       </c>
       <c r="M73" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="74" spans="1:13">
       <c r="A74">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B74" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C74">
-        <v>15612</v>
+        <v>18109</v>
       </c>
       <c r="D74">
-        <v>2445</v>
+        <v>222</v>
       </c>
       <c r="E74">
-        <v>234</v>
+        <v>255</v>
       </c>
       <c r="F74">
-        <v>10111</v>
+        <v>14314</v>
       </c>
       <c r="G74">
-        <v>2667</v>
+        <v>3250</v>
       </c>
       <c r="H74">
-        <v>155</v>
+        <v>68</v>
       </c>
       <c r="I74" s="12">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="J74" s="14">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="K74">
         <f>(I74/C74)*10000</f>
-        <v>22.418652318729183</v>
+        <v>2.7610580374399469</v>
       </c>
       <c r="L74">
         <f>(J74/C74)*10000</f>
-        <v>0.64053292339226231</v>
+        <v>11.596443757247776</v>
       </c>
       <c r="M74" t="s">
         <v>174</v>
@@ -7873,42 +7878,42 @@
     </row>
     <row r="75" spans="1:13">
       <c r="A75">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B75" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C75">
-        <v>37023</v>
+        <v>18508</v>
       </c>
       <c r="D75">
-        <v>1696</v>
+        <v>1989</v>
       </c>
       <c r="E75">
-        <v>164</v>
+        <v>137</v>
       </c>
       <c r="F75">
-        <v>4442</v>
+        <v>2126</v>
       </c>
       <c r="G75">
-        <v>30157</v>
+        <v>13815</v>
       </c>
       <c r="H75">
-        <v>564</v>
+        <v>441</v>
       </c>
       <c r="I75" s="12">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="J75" s="14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K75">
         <f>(I75/C75)*10000</f>
-        <v>3.2412284255732922</v>
+        <v>2.1612275772638858</v>
       </c>
       <c r="L75">
         <f>(J75/C75)*10000</f>
-        <v>1.0804094751910973</v>
+        <v>1.0806137886319429</v>
       </c>
       <c r="M75" t="s">
         <v>175</v>
@@ -7916,42 +7921,42 @@
     </row>
     <row r="76" spans="1:13">
       <c r="A76">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B76" t="s">
-        <v>11</v>
+        <v>84</v>
       </c>
       <c r="C76">
-        <v>18508</v>
+        <v>11187</v>
       </c>
       <c r="D76">
-        <v>1989</v>
+        <v>269</v>
       </c>
       <c r="E76">
-        <v>137</v>
+        <v>29</v>
       </c>
       <c r="F76">
-        <v>2126</v>
+        <v>872</v>
       </c>
       <c r="G76">
-        <v>13815</v>
+        <v>9885</v>
       </c>
       <c r="H76">
-        <v>441</v>
+        <v>132</v>
       </c>
       <c r="I76" s="12">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J76" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K76">
         <f>(I76/C76)*10000</f>
-        <v>2.1612275772638858</v>
+        <v>1.7877893984088675</v>
       </c>
       <c r="L76">
         <f>(J76/C76)*10000</f>
-        <v>1.0806137886319429</v>
+        <v>0.89389469920443376</v>
       </c>
       <c r="M76" t="s">
         <v>175</v>
@@ -7959,91 +7964,86 @@
     </row>
     <row r="77" spans="1:13">
       <c r="A77">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>167</v>
+        <v>81</v>
       </c>
       <c r="C77">
-        <v>13393</v>
+        <v>12756</v>
       </c>
       <c r="D77">
-        <v>138</v>
+        <v>1058</v>
       </c>
       <c r="E77">
-        <v>130</v>
+        <v>403</v>
       </c>
       <c r="F77">
-        <v>10182</v>
+        <v>1212</v>
       </c>
       <c r="G77">
-        <v>2874</v>
+        <v>9845</v>
       </c>
       <c r="H77">
-        <v>69</v>
+        <v>238</v>
       </c>
       <c r="I77" s="12">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="J77" s="15"/>
       <c r="K77">
         <f>(I77/C77)*10000</f>
-        <v>5.2266109161502277</v>
+        <v>0.7839448102853559</v>
       </c>
       <c r="L77">
         <f>(J77/C77)*10000</f>
         <v>0</v>
       </c>
       <c r="M77" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="78" spans="1:13">
       <c r="A78">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B78" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="C78">
-        <v>11187</v>
+        <v>13426</v>
       </c>
       <c r="D78">
-        <v>269</v>
+        <v>377</v>
       </c>
       <c r="E78">
-        <v>29</v>
+        <v>598</v>
       </c>
       <c r="F78">
-        <v>872</v>
+        <v>7248</v>
       </c>
       <c r="G78">
-        <v>9885</v>
+        <v>5041</v>
       </c>
       <c r="H78">
-        <v>132</v>
-      </c>
-      <c r="I78" s="12">
-        <v>2</v>
-      </c>
-      <c r="J78" s="12">
-        <v>1</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="J78" s="16"/>
       <c r="K78">
         <f>(I78/C78)*10000</f>
-        <v>1.7877893984088675</v>
+        <v>0</v>
       </c>
       <c r="L78">
         <f>(J78/C78)*10000</f>
-        <v>0.89389469920443376</v>
+        <v>0</v>
       </c>
       <c r="M78" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="A2:M78">
-    <sortCondition descending="1" ref="E2:E78"/>
+    <sortCondition descending="1" ref="K2:K78"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>